<commit_message>
Wow Controller added for getting woow through wow API
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -24,184 +24,184 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Lucious</t>
-  </si>
-  <si>
-    <t>East Ethylberg</t>
-  </si>
-  <si>
-    <t>West Edgar</t>
-  </si>
-  <si>
-    <t>Dallin</t>
-  </si>
-  <si>
-    <t>South Junior</t>
-  </si>
-  <si>
-    <t>Lake Izaiahmouth</t>
-  </si>
-  <si>
-    <t>Savannah</t>
-  </si>
-  <si>
-    <t>North Myrnaberg</t>
-  </si>
-  <si>
-    <t>Lake Bethanymouth</t>
-  </si>
-  <si>
-    <t>Raymundo</t>
-  </si>
-  <si>
-    <t>North Muhammad</t>
-  </si>
-  <si>
-    <t>Lake Cleo</t>
-  </si>
-  <si>
-    <t>Kurt</t>
-  </si>
-  <si>
-    <t>West Reggiefurt</t>
-  </si>
-  <si>
-    <t>Revaville</t>
-  </si>
-  <si>
-    <t>Aliya</t>
-  </si>
-  <si>
-    <t>Satterfieldton</t>
-  </si>
-  <si>
-    <t>Lake Oma</t>
-  </si>
-  <si>
-    <t>Jaunita</t>
-  </si>
-  <si>
-    <t>New Lilly</t>
-  </si>
-  <si>
-    <t>Brekkefort</t>
-  </si>
-  <si>
-    <t>Einar</t>
-  </si>
-  <si>
-    <t>Boyertown</t>
-  </si>
-  <si>
-    <t>South Bria</t>
-  </si>
-  <si>
-    <t>Kiana</t>
-  </si>
-  <si>
-    <t>Stokeston</t>
-  </si>
-  <si>
-    <t>East Dasiaport</t>
-  </si>
-  <si>
-    <t>Zachery</t>
-  </si>
-  <si>
-    <t>Eduardoland</t>
-  </si>
-  <si>
-    <t>Streichville</t>
-  </si>
-  <si>
-    <t>Victoria</t>
-  </si>
-  <si>
-    <t>Vanessahaven</t>
-  </si>
-  <si>
-    <t>Lake Evertfurt</t>
-  </si>
-  <si>
-    <t>Agustin</t>
-  </si>
-  <si>
-    <t>Jenkinsborough</t>
-  </si>
-  <si>
-    <t>Wileyborough</t>
-  </si>
-  <si>
-    <t>Lorenzo</t>
-  </si>
-  <si>
-    <t>Johanchester</t>
-  </si>
-  <si>
-    <t>West Mossieshire</t>
-  </si>
-  <si>
-    <t>Armand</t>
-  </si>
-  <si>
-    <t>Schowaltermouth</t>
-  </si>
-  <si>
-    <t>Bradtkeborough</t>
-  </si>
-  <si>
-    <t>Benedict</t>
-  </si>
-  <si>
-    <t>South Cordell</t>
-  </si>
-  <si>
-    <t>South Era</t>
-  </si>
-  <si>
-    <t>Annabell</t>
-  </si>
-  <si>
-    <t>North Gabrielle</t>
-  </si>
-  <si>
-    <t>Hahnbury</t>
-  </si>
-  <si>
-    <t>Elisa</t>
-  </si>
-  <si>
-    <t>New Demarcusville</t>
-  </si>
-  <si>
-    <t>Adonisstad</t>
-  </si>
-  <si>
-    <t>Retha</t>
-  </si>
-  <si>
-    <t>Lake Rosendo</t>
-  </si>
-  <si>
-    <t>Christiansenborough</t>
-  </si>
-  <si>
-    <t>Tyrique</t>
-  </si>
-  <si>
-    <t>West Sabrina</t>
-  </si>
-  <si>
-    <t>South Bennie</t>
-  </si>
-  <si>
-    <t>Forest</t>
-  </si>
-  <si>
-    <t>West Marquistown</t>
-  </si>
-  <si>
-    <t>East Dillanstad</t>
+    <t>Carrie</t>
+  </si>
+  <si>
+    <t>Wellingtonton</t>
+  </si>
+  <si>
+    <t>Erdmanview</t>
+  </si>
+  <si>
+    <t>Larissa</t>
+  </si>
+  <si>
+    <t>Mannview</t>
+  </si>
+  <si>
+    <t>Gleasonmouth</t>
+  </si>
+  <si>
+    <t>Colten</t>
+  </si>
+  <si>
+    <t>Nicolasfort</t>
+  </si>
+  <si>
+    <t>Beckerland</t>
+  </si>
+  <si>
+    <t>Hettie</t>
+  </si>
+  <si>
+    <t>Lake Floy</t>
+  </si>
+  <si>
+    <t>North Ernestine</t>
+  </si>
+  <si>
+    <t>Mittie</t>
+  </si>
+  <si>
+    <t>Jacobsonbury</t>
+  </si>
+  <si>
+    <t>Willburgh</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>North Hillardburgh</t>
+  </si>
+  <si>
+    <t>Kaialand</t>
+  </si>
+  <si>
+    <t>Stan</t>
+  </si>
+  <si>
+    <t>Lake Karelle</t>
+  </si>
+  <si>
+    <t>West Elza</t>
+  </si>
+  <si>
+    <t>Heath</t>
+  </si>
+  <si>
+    <t>Katherynchester</t>
+  </si>
+  <si>
+    <t>Karianefurt</t>
+  </si>
+  <si>
+    <t>Rosina</t>
+  </si>
+  <si>
+    <t>Rempelland</t>
+  </si>
+  <si>
+    <t>East Ward</t>
+  </si>
+  <si>
+    <t>Terrell</t>
+  </si>
+  <si>
+    <t>West Carley</t>
+  </si>
+  <si>
+    <t>Kylerburgh</t>
+  </si>
+  <si>
+    <t>Walton</t>
+  </si>
+  <si>
+    <t>Westmouth</t>
+  </si>
+  <si>
+    <t>Genesisview</t>
+  </si>
+  <si>
+    <t>Hassie</t>
+  </si>
+  <si>
+    <t>East Andreane</t>
+  </si>
+  <si>
+    <t>Faheytown</t>
+  </si>
+  <si>
+    <t>Beau</t>
+  </si>
+  <si>
+    <t>Kutchview</t>
+  </si>
+  <si>
+    <t>Lake Alysa</t>
+  </si>
+  <si>
+    <t>Hollie</t>
+  </si>
+  <si>
+    <t>Halvorsonbury</t>
+  </si>
+  <si>
+    <t>Elysehaven</t>
+  </si>
+  <si>
+    <t>Alden</t>
+  </si>
+  <si>
+    <t>Lake Tylermouth</t>
+  </si>
+  <si>
+    <t>Wiegandfort</t>
+  </si>
+  <si>
+    <t>Neva</t>
+  </si>
+  <si>
+    <t>South Susan</t>
+  </si>
+  <si>
+    <t>Conroyhaven</t>
+  </si>
+  <si>
+    <t>Era</t>
+  </si>
+  <si>
+    <t>East Krystinaside</t>
+  </si>
+  <si>
+    <t>Monahanland</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Lake Fannie</t>
+  </si>
+  <si>
+    <t>Goldnerside</t>
+  </si>
+  <si>
+    <t>Violet</t>
+  </si>
+  <si>
+    <t>New Jordy</t>
+  </si>
+  <si>
+    <t>New Wilbertberg</t>
+  </si>
+  <si>
+    <t>Madyson</t>
+  </si>
+  <si>
+    <t>Bayershire</t>
+  </si>
+  <si>
+    <t>Jerodland</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
COMMIT FROM SOURE TREE 0001
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -24,184 +24,184 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Gino</t>
-  </si>
-  <si>
-    <t>East Roryborough</t>
-  </si>
-  <si>
-    <t>New Chantellberg</t>
-  </si>
-  <si>
-    <t>Sulema</t>
-  </si>
-  <si>
-    <t>North Molly</t>
-  </si>
-  <si>
-    <t>Clydeburgh</t>
-  </si>
-  <si>
-    <t>Providencia</t>
-  </si>
-  <si>
-    <t>West Corey</t>
-  </si>
-  <si>
-    <t>Herzogstad</t>
-  </si>
-  <si>
-    <t>Sean</t>
-  </si>
-  <si>
-    <t>Yundtfurt</t>
-  </si>
-  <si>
-    <t>South Jerrieville</t>
-  </si>
-  <si>
-    <t>Winfred</t>
-  </si>
-  <si>
-    <t>Jodeechester</t>
-  </si>
-  <si>
-    <t>Lake Berta</t>
-  </si>
-  <si>
-    <t>Joan</t>
-  </si>
-  <si>
-    <t>Blakemouth</t>
-  </si>
-  <si>
-    <t>Irvinview</t>
-  </si>
-  <si>
-    <t>Emeline</t>
-  </si>
-  <si>
-    <t>West Joan</t>
-  </si>
-  <si>
-    <t>East Cathrynburgh</t>
-  </si>
-  <si>
-    <t>Franklin</t>
-  </si>
-  <si>
-    <t>Walkershire</t>
-  </si>
-  <si>
-    <t>Herbport</t>
-  </si>
-  <si>
-    <t>Eduardo</t>
-  </si>
-  <si>
-    <t>South Jerald</t>
-  </si>
-  <si>
-    <t>Byronside</t>
-  </si>
-  <si>
-    <t>Leslie</t>
-  </si>
-  <si>
-    <t>South Rodgerberg</t>
-  </si>
-  <si>
-    <t>North Daleburgh</t>
-  </si>
-  <si>
-    <t>Anton</t>
-  </si>
-  <si>
-    <t>Melinafurt</t>
-  </si>
-  <si>
-    <t>Kemmertown</t>
-  </si>
-  <si>
-    <t>Arlie</t>
-  </si>
-  <si>
-    <t>Runolfssonside</t>
-  </si>
-  <si>
-    <t>Stefanyland</t>
-  </si>
-  <si>
-    <t>Kerry</t>
-  </si>
-  <si>
-    <t>Pamelialand</t>
-  </si>
-  <si>
-    <t>Lake Martine</t>
-  </si>
-  <si>
-    <t>Hank</t>
-  </si>
-  <si>
-    <t>Lake Tiffaniehaven</t>
-  </si>
-  <si>
-    <t>South Lacyside</t>
-  </si>
-  <si>
-    <t>Alejandrina</t>
-  </si>
-  <si>
-    <t>Brandeside</t>
-  </si>
-  <si>
-    <t>West Octavio</t>
-  </si>
-  <si>
-    <t>Tanya</t>
-  </si>
-  <si>
-    <t>West Huongview</t>
-  </si>
-  <si>
-    <t>Wehnerstad</t>
-  </si>
-  <si>
-    <t>Jerry</t>
-  </si>
-  <si>
-    <t>Murrayfort</t>
-  </si>
-  <si>
-    <t>Rosaside</t>
-  </si>
-  <si>
-    <t>Ernest</t>
-  </si>
-  <si>
-    <t>New Petra</t>
-  </si>
-  <si>
-    <t>Zacharychester</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Lake Robert</t>
-  </si>
-  <si>
-    <t>Port Yuk</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>Deirdremouth</t>
-  </si>
-  <si>
-    <t>South Lisbethville</t>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Weberburgh</t>
+  </si>
+  <si>
+    <t>Port Ursulachester</t>
+  </si>
+  <si>
+    <t>Geoffrey</t>
+  </si>
+  <si>
+    <t>East Delois</t>
+  </si>
+  <si>
+    <t>New Arnold</t>
+  </si>
+  <si>
+    <t>Ariane</t>
+  </si>
+  <si>
+    <t>Port Vernitaburgh</t>
+  </si>
+  <si>
+    <t>Cheyenneton</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>Heathcoteberg</t>
+  </si>
+  <si>
+    <t>Sonnychester</t>
+  </si>
+  <si>
+    <t>Gussie</t>
+  </si>
+  <si>
+    <t>Wintheiserview</t>
+  </si>
+  <si>
+    <t>Jessemouth</t>
+  </si>
+  <si>
+    <t>Etsuko</t>
+  </si>
+  <si>
+    <t>Beverleyville</t>
+  </si>
+  <si>
+    <t>North Porfirio</t>
+  </si>
+  <si>
+    <t>Lorita</t>
+  </si>
+  <si>
+    <t>South Winfordtown</t>
+  </si>
+  <si>
+    <t>East Vito</t>
+  </si>
+  <si>
+    <t>Dessie</t>
+  </si>
+  <si>
+    <t>East Laynefurt</t>
+  </si>
+  <si>
+    <t>Amaliaberg</t>
+  </si>
+  <si>
+    <t>Rosalie</t>
+  </si>
+  <si>
+    <t>Rodrickmouth</t>
+  </si>
+  <si>
+    <t>Lake Kyrabury</t>
+  </si>
+  <si>
+    <t>Andria</t>
+  </si>
+  <si>
+    <t>Kayebury</t>
+  </si>
+  <si>
+    <t>Wisokyborough</t>
+  </si>
+  <si>
+    <t>Horace</t>
+  </si>
+  <si>
+    <t>Langstad</t>
+  </si>
+  <si>
+    <t>Nikolausmouth</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>Port Jeninetown</t>
+  </si>
+  <si>
+    <t>Abernathyville</t>
+  </si>
+  <si>
+    <t>Jettie</t>
+  </si>
+  <si>
+    <t>Kovacekhaven</t>
+  </si>
+  <si>
+    <t>Port Bennie</t>
+  </si>
+  <si>
+    <t>Delmy</t>
+  </si>
+  <si>
+    <t>Port Valorie</t>
+  </si>
+  <si>
+    <t>East Denis</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>East Vitoburgh</t>
+  </si>
+  <si>
+    <t>Jacqulynfort</t>
+  </si>
+  <si>
+    <t>Jung</t>
+  </si>
+  <si>
+    <t>Howebury</t>
+  </si>
+  <si>
+    <t>East Annie</t>
+  </si>
+  <si>
+    <t>Beverlee</t>
+  </si>
+  <si>
+    <t>Port Haibury</t>
+  </si>
+  <si>
+    <t>Mollytown</t>
+  </si>
+  <si>
+    <t>Cornell</t>
+  </si>
+  <si>
+    <t>Goldnerview</t>
+  </si>
+  <si>
+    <t>East Fidelberg</t>
+  </si>
+  <si>
+    <t>Twanna</t>
+  </si>
+  <si>
+    <t>Wintheiserborough</t>
+  </si>
+  <si>
+    <t>Neliatown</t>
+  </si>
+  <si>
+    <t>Young</t>
+  </si>
+  <si>
+    <t>West Bernettachester</t>
+  </si>
+  <si>
+    <t>West Modestafort</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Spring data jpa is added
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -24,184 +24,184 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Stephen</t>
-  </si>
-  <si>
-    <t>Weberburgh</t>
-  </si>
-  <si>
-    <t>Port Ursulachester</t>
-  </si>
-  <si>
-    <t>Geoffrey</t>
-  </si>
-  <si>
-    <t>East Delois</t>
-  </si>
-  <si>
-    <t>New Arnold</t>
-  </si>
-  <si>
-    <t>Ariane</t>
-  </si>
-  <si>
-    <t>Port Vernitaburgh</t>
-  </si>
-  <si>
-    <t>Cheyenneton</t>
-  </si>
-  <si>
-    <t>Troy</t>
-  </si>
-  <si>
-    <t>Heathcoteberg</t>
-  </si>
-  <si>
-    <t>Sonnychester</t>
-  </si>
-  <si>
-    <t>Gussie</t>
-  </si>
-  <si>
-    <t>Wintheiserview</t>
-  </si>
-  <si>
-    <t>Jessemouth</t>
-  </si>
-  <si>
-    <t>Etsuko</t>
-  </si>
-  <si>
-    <t>Beverleyville</t>
-  </si>
-  <si>
-    <t>North Porfirio</t>
-  </si>
-  <si>
-    <t>Lorita</t>
-  </si>
-  <si>
-    <t>South Winfordtown</t>
-  </si>
-  <si>
-    <t>East Vito</t>
-  </si>
-  <si>
-    <t>Dessie</t>
-  </si>
-  <si>
-    <t>East Laynefurt</t>
-  </si>
-  <si>
-    <t>Amaliaberg</t>
-  </si>
-  <si>
-    <t>Rosalie</t>
-  </si>
-  <si>
-    <t>Rodrickmouth</t>
-  </si>
-  <si>
-    <t>Lake Kyrabury</t>
-  </si>
-  <si>
-    <t>Andria</t>
-  </si>
-  <si>
-    <t>Kayebury</t>
-  </si>
-  <si>
-    <t>Wisokyborough</t>
-  </si>
-  <si>
-    <t>Horace</t>
-  </si>
-  <si>
-    <t>Langstad</t>
-  </si>
-  <si>
-    <t>Nikolausmouth</t>
-  </si>
-  <si>
-    <t>Ralph</t>
-  </si>
-  <si>
-    <t>Port Jeninetown</t>
-  </si>
-  <si>
-    <t>Abernathyville</t>
-  </si>
-  <si>
-    <t>Jettie</t>
-  </si>
-  <si>
-    <t>Kovacekhaven</t>
-  </si>
-  <si>
-    <t>Port Bennie</t>
-  </si>
-  <si>
-    <t>Delmy</t>
-  </si>
-  <si>
-    <t>Port Valorie</t>
-  </si>
-  <si>
-    <t>East Denis</t>
-  </si>
-  <si>
-    <t>Santiago</t>
-  </si>
-  <si>
-    <t>East Vitoburgh</t>
-  </si>
-  <si>
-    <t>Jacqulynfort</t>
-  </si>
-  <si>
-    <t>Jung</t>
-  </si>
-  <si>
-    <t>Howebury</t>
-  </si>
-  <si>
-    <t>East Annie</t>
-  </si>
-  <si>
-    <t>Beverlee</t>
-  </si>
-  <si>
-    <t>Port Haibury</t>
-  </si>
-  <si>
-    <t>Mollytown</t>
-  </si>
-  <si>
-    <t>Cornell</t>
-  </si>
-  <si>
-    <t>Goldnerview</t>
-  </si>
-  <si>
-    <t>East Fidelberg</t>
-  </si>
-  <si>
-    <t>Twanna</t>
-  </si>
-  <si>
-    <t>Wintheiserborough</t>
-  </si>
-  <si>
-    <t>Neliatown</t>
-  </si>
-  <si>
-    <t>Young</t>
-  </si>
-  <si>
-    <t>West Bernettachester</t>
-  </si>
-  <si>
-    <t>West Modestafort</t>
+    <t>Frederick</t>
+  </si>
+  <si>
+    <t>Hoegerhaven</t>
+  </si>
+  <si>
+    <t>Robertsville</t>
+  </si>
+  <si>
+    <t>Pilar</t>
+  </si>
+  <si>
+    <t>Ankundinghaven</t>
+  </si>
+  <si>
+    <t>Port Alishatown</t>
+  </si>
+  <si>
+    <t>Carma</t>
+  </si>
+  <si>
+    <t>North Roderickton</t>
+  </si>
+  <si>
+    <t>Bergnaumport</t>
+  </si>
+  <si>
+    <t>Shan</t>
+  </si>
+  <si>
+    <t>Abeview</t>
+  </si>
+  <si>
+    <t>New Jenineburgh</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Kuhicmouth</t>
+  </si>
+  <si>
+    <t>Labadiemouth</t>
+  </si>
+  <si>
+    <t>Niki</t>
+  </si>
+  <si>
+    <t>Powlowskifort</t>
+  </si>
+  <si>
+    <t>North Joline</t>
+  </si>
+  <si>
+    <t>Charis</t>
+  </si>
+  <si>
+    <t>South Toryburgh</t>
+  </si>
+  <si>
+    <t>West Devonside</t>
+  </si>
+  <si>
+    <t>Eugene</t>
+  </si>
+  <si>
+    <t>Lake Vincenzo</t>
+  </si>
+  <si>
+    <t>New Abbeyfurt</t>
+  </si>
+  <si>
+    <t>Gregorio</t>
+  </si>
+  <si>
+    <t>Rolfsonland</t>
+  </si>
+  <si>
+    <t>Port Nikoleland</t>
+  </si>
+  <si>
+    <t>Carlena</t>
+  </si>
+  <si>
+    <t>Marielberg</t>
+  </si>
+  <si>
+    <t>Breitenbergfurt</t>
+  </si>
+  <si>
+    <t>Mack</t>
+  </si>
+  <si>
+    <t>Sporerside</t>
+  </si>
+  <si>
+    <t>Hueport</t>
+  </si>
+  <si>
+    <t>Alica</t>
+  </si>
+  <si>
+    <t>Stefanmouth</t>
+  </si>
+  <si>
+    <t>Hughshire</t>
+  </si>
+  <si>
+    <t>Jesenia</t>
+  </si>
+  <si>
+    <t>Lake Marylee</t>
+  </si>
+  <si>
+    <t>Port Elizbeth</t>
+  </si>
+  <si>
+    <t>Dianna</t>
+  </si>
+  <si>
+    <t>Thanhstad</t>
+  </si>
+  <si>
+    <t>South Renaymouth</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>South Clemente</t>
+  </si>
+  <si>
+    <t>Scarletthaven</t>
+  </si>
+  <si>
+    <t>Cristopher</t>
+  </si>
+  <si>
+    <t>Shawntaside</t>
+  </si>
+  <si>
+    <t>Port Mirellaview</t>
+  </si>
+  <si>
+    <t>Rebecka</t>
+  </si>
+  <si>
+    <t>North Keira</t>
+  </si>
+  <si>
+    <t>East Sherell</t>
+  </si>
+  <si>
+    <t>Leopoldo</t>
+  </si>
+  <si>
+    <t>Jeremymouth</t>
+  </si>
+  <si>
+    <t>South Naoma</t>
+  </si>
+  <si>
+    <t>Gabriella</t>
+  </si>
+  <si>
+    <t>Lockmanbury</t>
+  </si>
+  <si>
+    <t>North Libbyfurt</t>
+  </si>
+  <si>
+    <t>Silvana</t>
+  </si>
+  <si>
+    <t>Lake Stuartmouth</t>
+  </si>
+  <si>
+    <t>South Terrell</t>
   </si>
 </sst>
 </file>

</xml_diff>